<commit_message>
pakn de tests finito et affichage msg derreur
</commit_message>
<xml_diff>
--- a/Template+de+Plan+de+tests.xlsx
+++ b/Template+de+Plan+de+tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmca\Desktop\open c\EmmaCariot_5_18062021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC510201-EE74-4C0C-AC07-817F99CDCB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF69DA-9DB2-4D6E-99DD-3286BD16DA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -109,7 +109,94 @@
     <t>addToLocalStorage</t>
   </si>
   <si>
-    <t xml:space="preserve">La fonction créé un tableau de produits dans lequel se trouve tous les oursons selectionnés. Si le LS existe déjà, on ajoute les oursons selectionnés en plus. S'il n'existe pas, on le créé. </t>
+    <t xml:space="preserve">La fonction créé un tableau de produits dans lequel se trouve tous les oursons selectionnés. Si le LS existe déjà, on ajoute les oursons selectionnés en plus. S'il n'existe pas, on le créé. Sert aussi à convertir la valeur JS en chaîne de caractère JSON. Ce qui est essentiel pour le local storage.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ouvrir la console puis aller dans Application. Regarder si on a tous les id des oursons selectionnés. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La gestion de la quantité. Il faut que les mêmes id soient dans le même tableau. Il ne faut pas que ça se transforme en un id un produit. </t>
+  </si>
+  <si>
+    <t>cart.js</t>
+  </si>
+  <si>
+    <t>13 à 50</t>
+  </si>
+  <si>
+    <t>displayCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction créé des divs pour afficher toutes les précisions du panier. Création de section pour le nom de l'ours, le prix la quantité et l'option de supprimer le produit. </t>
+  </si>
+  <si>
+    <t>Regarder sur la page panier si tout se met au bon endroit. Et si plusieurs mêmes oursons sont selectionés, qu'ils se mettent sur la même ligne. Regarder si le bouton supprimer, supprime bien du local storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que le même produit s'affiche sur plusieurs lignes car il a été sélectionné plusieurs fois. Ou alors qu'un produit ne se supprime pas. </t>
+  </si>
+  <si>
+    <t>52 à 59</t>
+  </si>
+  <si>
+    <t>displayTotal</t>
+  </si>
+  <si>
+    <t>Fonction qui permet d'afficher le total de la commande. C'est dynamique donc il s'actualise lorsqu'un produit est ajouté ou supprimé. On vient multiplier les "price" des oursons avec lesquels on a travaillé dans displayCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire un rapide calcul et se rendre compte si la multiplcation a bien été faite. Faire les tests avec le bouton supprimer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S'il y a plusieurs mêmes oursons selcetionnés, que le total ne se fasse que sur un seul. </t>
+  </si>
+  <si>
+    <t>61 à 67</t>
+  </si>
+  <si>
+    <t>clearCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction sert à vider le panier. On fait donc un addvenlistener sur le bouton "vider le panier". Et tous les articles précedemment sélectionnés doivent être supprimés. </t>
+  </si>
+  <si>
+    <t>Voir que la page de panier s'actualise sans aucun produit. Et regarder si le LS est bien vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que le panier se vide en théorie sur la page. Mais que le Local storage reste plein. </t>
+  </si>
+  <si>
+    <t>69 à 118</t>
+  </si>
+  <si>
+    <t>postRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction sert à faire une requête post pour envoyer les données de contact et d'id à L'API. On récupère les informations du Dom qui sont demandées. L'ortographe doit bien être similaire à celle demandée par le back end. Cf les fichiers backend. On créé un objet de contact avec toutes les informations du client. Puis on créé un tableau avec les id des oursons. On utilise par la suite la méthode POST avecc FETCH. Cette requête contient le contact du client et les id des oursons. Ceci est contenu dans l'objet options. Puis on redirige vers la page de confirmation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aller dans la console et se rendre compte de si tous les tableaux ont bien été crées. Si tout est conforme, la page de confirmation doit afficher un numéro de commande. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire très attention à l'ortographe des obejts et des valeurs. Sinon la requête est mauvaise. Et la fin du processus ne peut pas se faire. </t>
+  </si>
+  <si>
+    <t>confirmation.js</t>
+  </si>
+  <si>
+    <t>1 à 9</t>
+  </si>
+  <si>
+    <t>displayOrderId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction affiche le numéro d'id de la commande. Et vide le Local Storage pour recommencer le processus d'achat. Après la requête post, le backend nous renvoie l'id de la commande si les objets envoyés étaient bons. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afficher sur une page une div qui contient l'orderID. S'il y a marqué undifined c'est qu'il y a un problème. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que le local storage ne se vide pas et que cela perturbe le prochain processus d'achat. </t>
   </si>
 </sst>
 </file>
@@ -400,9 +487,9 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -553,33 +640,112 @@
       <c r="D7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>

</xml_diff>